<commit_message>
Changing spec to specify appendCodeName for curveid
</commit_message>
<xml_diff>
--- a/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
+++ b/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="0" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2012-0703 herg upload for seura" sheetId="1" r:id="rId1"/>
@@ -35,30 +35,6 @@
             <family val="2"/>
           </rPr>
           <t>Allowed values are Number, Text, and Date. The loader will interpret blanks as Number.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Samuel Meyer:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Should links be recorded in the databse?</t>
         </r>
       </text>
     </comment>
@@ -363,9 +339,6 @@
     <t>StateKind</t>
   </si>
   <si>
-    <t>Text [link]</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -415,6 +388,9 @@
   </si>
   <si>
     <t>Dose (uM); batch code</t>
+  </si>
+  <si>
+    <t>Text [link; appendCodeName]</t>
   </si>
 </sst>
 </file>
@@ -870,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -900,15 +876,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -927,7 +903,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -950,25 +926,25 @@
         <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -976,25 +952,25 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1340,31 +1316,31 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1393,7 +1369,7 @@
         <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1401,19 +1377,19 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1421,24 +1397,24 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1450,10 +1426,10 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2833,7 +2809,7 @@
         <v>81</v>
       </c>
       <c r="F113" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="114" spans="1:6">

</xml_diff>

<commit_message>
SEL: editing example code in comments at top
</commit_message>
<xml_diff>
--- a/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
+++ b/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="62">
   <si>
     <t>Format</t>
   </si>
@@ -253,12 +253,6 @@
   </si>
   <si>
     <t>Rendering Hint</t>
-  </si>
-  <si>
-    <t>CMPD-0000004-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000005-01</t>
   </si>
   <si>
     <t>Text</t>
@@ -310,27 +304,6 @@
   </si>
   <si>
     <t>CMPD-0000002-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000003-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000006-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000007-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000008-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000009-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000010-01</t>
-  </si>
-  <si>
-    <t>CMPD-0000011-01</t>
   </si>
   <si>
     <t>StateType</t>
@@ -391,6 +364,39 @@
   </si>
   <si>
     <t>Text [link; appendCodeName]</t>
+  </si>
+  <si>
+    <t>CMPD-0000001-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000002-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000003-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000004-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000005-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000006-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000007-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000008-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000009-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000010-01A</t>
+  </si>
+  <si>
+    <t>CMPD-0000011-01A</t>
   </si>
 </sst>
 </file>
@@ -491,10 +497,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,12 +516,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -847,7 +857,7 @@
   <dimension ref="A1:H432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -876,15 +886,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -900,77 +910,77 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -984,16 +994,16 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
@@ -1001,13 +1011,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>102.911</v>
@@ -1027,13 +1037,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -1053,13 +1063,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>100</v>
@@ -1079,13 +1089,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>100</v>
@@ -1105,13 +1115,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -1131,13 +1141,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -1157,7 +1167,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -1183,7 +1193,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1209,7 +1219,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1235,7 +1245,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -1261,7 +1271,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1287,7 +1297,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1316,31 +1326,31 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1357,64 +1367,64 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1426,15 +1436,15 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>20</v>
@@ -1446,12 +1456,12 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -1460,18 +1470,18 @@
         <v>89.825999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -1483,12 +1493,12 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B36">
         <v>2.5</v>
@@ -1500,12 +1510,12 @@
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37">
         <v>1.25</v>
@@ -1517,12 +1527,12 @@
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B38">
         <v>0.625</v>
@@ -1534,12 +1544,12 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39">
         <v>0.3125</v>
@@ -1551,12 +1561,12 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40">
         <v>0.15625</v>
@@ -1568,12 +1578,12 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B41">
         <v>7.8125E-2</v>
@@ -1585,12 +1595,12 @@
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <v>3.9063000000000001E-2</v>
@@ -1602,12 +1612,12 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B43">
         <v>20</v>
@@ -1619,12 +1629,12 @@
         <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B44">
         <v>10</v>
@@ -1636,12 +1646,12 @@
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B45">
         <v>5</v>
@@ -1653,12 +1663,12 @@
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B46">
         <v>2.5</v>
@@ -1670,12 +1680,12 @@
         <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B47">
         <v>1.25</v>
@@ -1687,12 +1697,12 @@
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48">
         <v>0.625</v>
@@ -1704,12 +1714,12 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B49">
         <v>0.3125</v>
@@ -1721,12 +1731,12 @@
         <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>0.15625</v>
@@ -1738,12 +1748,12 @@
         <v>18</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>7.8125E-2</v>
@@ -1755,12 +1765,12 @@
         <v>19</v>
       </c>
       <c r="F51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B52">
         <v>3.9063000000000001E-2</v>
@@ -1772,12 +1782,12 @@
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>20</v>
@@ -1789,12 +1799,12 @@
         <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B54">
         <v>10</v>
@@ -1806,12 +1816,12 @@
         <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -1823,12 +1833,12 @@
         <v>23</v>
       </c>
       <c r="F55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56">
         <v>2.5</v>
@@ -1840,12 +1850,12 @@
         <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B57">
         <v>1.25</v>
@@ -1857,12 +1867,12 @@
         <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B58">
         <v>0.625</v>
@@ -1874,12 +1884,12 @@
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B59">
         <v>0.3125</v>
@@ -1891,12 +1901,12 @@
         <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B60">
         <v>0.15625</v>
@@ -1908,12 +1918,12 @@
         <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B61">
         <v>7.8125E-2</v>
@@ -1925,12 +1935,12 @@
         <v>29</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B62">
         <v>3.9063000000000001E-2</v>
@@ -1942,12 +1952,12 @@
         <v>30</v>
       </c>
       <c r="F62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B63">
         <v>20</v>
@@ -1959,12 +1969,12 @@
         <v>31</v>
       </c>
       <c r="F63" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -1976,12 +1986,12 @@
         <v>32</v>
       </c>
       <c r="F64" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -1993,12 +2003,12 @@
         <v>33</v>
       </c>
       <c r="F65" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B66">
         <v>2.5</v>
@@ -2010,12 +2020,12 @@
         <v>34</v>
       </c>
       <c r="F66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B67">
         <v>1.25</v>
@@ -2027,12 +2037,12 @@
         <v>35</v>
       </c>
       <c r="F67" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B68">
         <v>0.625</v>
@@ -2044,12 +2054,12 @@
         <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B69">
         <v>0.3125</v>
@@ -2061,12 +2071,12 @@
         <v>37</v>
       </c>
       <c r="F69" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B70">
         <v>0.15625</v>
@@ -2078,12 +2088,12 @@
         <v>38</v>
       </c>
       <c r="F70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B71">
         <v>7.8125E-2</v>
@@ -2095,12 +2105,12 @@
         <v>39</v>
       </c>
       <c r="F71" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B72">
         <v>3.9063000000000001E-2</v>
@@ -2112,12 +2122,12 @@
         <v>40</v>
       </c>
       <c r="F72" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B73">
         <v>0.3125</v>
@@ -2129,12 +2139,12 @@
         <v>41</v>
       </c>
       <c r="F73" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B74">
         <v>0.15625</v>
@@ -2146,12 +2156,12 @@
         <v>42</v>
       </c>
       <c r="F74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B75">
         <v>7.8125E-2</v>
@@ -2163,12 +2173,12 @@
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B76">
         <v>3.9063000000000001E-2</v>
@@ -2180,12 +2190,12 @@
         <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B77">
         <v>20</v>
@@ -2197,12 +2207,12 @@
         <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B78">
         <v>10</v>
@@ -2214,12 +2224,12 @@
         <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B79">
         <v>5</v>
@@ -2231,12 +2241,12 @@
         <v>47</v>
       </c>
       <c r="F79" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B80">
         <v>2.5</v>
@@ -2248,12 +2258,12 @@
         <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B81">
         <v>1.25</v>
@@ -2265,12 +2275,12 @@
         <v>49</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B82">
         <v>0.625</v>
@@ -2282,12 +2292,12 @@
         <v>50</v>
       </c>
       <c r="F82" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B83">
         <v>0.3125</v>
@@ -2299,12 +2309,12 @@
         <v>51</v>
       </c>
       <c r="F83" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84">
         <v>0.15625</v>
@@ -2316,12 +2326,12 @@
         <v>52</v>
       </c>
       <c r="F84" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B85">
         <v>7.8125E-2</v>
@@ -2333,12 +2343,12 @@
         <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B86">
         <v>3.9063000000000001E-2</v>
@@ -2350,12 +2360,12 @@
         <v>54</v>
       </c>
       <c r="F86" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B87">
         <v>20</v>
@@ -2367,12 +2377,12 @@
         <v>55</v>
       </c>
       <c r="F87" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B88">
         <v>10</v>
@@ -2384,12 +2394,12 @@
         <v>56</v>
       </c>
       <c r="F88" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B89">
         <v>5</v>
@@ -2401,12 +2411,12 @@
         <v>57</v>
       </c>
       <c r="F89" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B90">
         <v>2.5</v>
@@ -2418,12 +2428,12 @@
         <v>58</v>
       </c>
       <c r="F90" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B91">
         <v>1.25</v>
@@ -2435,12 +2445,12 @@
         <v>59</v>
       </c>
       <c r="F91" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B92">
         <v>0.625</v>
@@ -2452,12 +2462,12 @@
         <v>60</v>
       </c>
       <c r="F92" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B93">
         <v>0.3125</v>
@@ -2469,12 +2479,12 @@
         <v>61</v>
       </c>
       <c r="F93" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B94">
         <v>0.15625</v>
@@ -2486,12 +2496,12 @@
         <v>62</v>
       </c>
       <c r="F94" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B95">
         <v>7.8125E-2</v>
@@ -2503,12 +2513,12 @@
         <v>63</v>
       </c>
       <c r="F95" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B96">
         <v>3.9063000000000001E-2</v>
@@ -2520,12 +2530,12 @@
         <v>64</v>
       </c>
       <c r="F96" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B97">
         <v>20</v>
@@ -2537,12 +2547,12 @@
         <v>65</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B98">
         <v>10</v>
@@ -2554,12 +2564,12 @@
         <v>66</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B99">
         <v>5</v>
@@ -2571,12 +2581,12 @@
         <v>67</v>
       </c>
       <c r="F99" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B100">
         <v>2.5</v>
@@ -2588,12 +2598,12 @@
         <v>68</v>
       </c>
       <c r="F100" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B101">
         <v>1.25</v>
@@ -2605,12 +2615,12 @@
         <v>69</v>
       </c>
       <c r="F101" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B102">
         <v>0.625</v>
@@ -2622,12 +2632,12 @@
         <v>70</v>
       </c>
       <c r="F102" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B103">
         <v>0.3125</v>
@@ -2639,12 +2649,12 @@
         <v>71</v>
       </c>
       <c r="F103" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B104">
         <v>0.15625</v>
@@ -2656,12 +2666,12 @@
         <v>72</v>
       </c>
       <c r="F104" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B105">
         <v>7.8125E-2</v>
@@ -2673,12 +2683,12 @@
         <v>73</v>
       </c>
       <c r="F105" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B106">
         <v>3.9063000000000001E-2</v>
@@ -2690,12 +2700,12 @@
         <v>74</v>
       </c>
       <c r="F106" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B107">
         <v>20</v>
@@ -2707,12 +2717,12 @@
         <v>75</v>
       </c>
       <c r="F107" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B108">
         <v>10</v>
@@ -2724,12 +2734,12 @@
         <v>76</v>
       </c>
       <c r="F108" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B109">
         <v>5</v>
@@ -2741,12 +2751,12 @@
         <v>77</v>
       </c>
       <c r="F109" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B110">
         <v>2.5</v>
@@ -2758,12 +2768,12 @@
         <v>78</v>
       </c>
       <c r="F110" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B111">
         <v>1.25</v>
@@ -2775,12 +2785,12 @@
         <v>79</v>
       </c>
       <c r="F111" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B112">
         <v>0.625</v>
@@ -2792,12 +2802,12 @@
         <v>80</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B113">
         <v>20</v>
@@ -2809,12 +2819,12 @@
         <v>81</v>
       </c>
       <c r="F113" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B114">
         <v>10</v>
@@ -2828,7 +2838,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B115">
         <v>5</v>
@@ -2842,7 +2852,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B116">
         <v>2.5</v>
@@ -2856,7 +2866,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B117">
         <v>1.25</v>
@@ -2870,7 +2880,7 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B118">
         <v>0.625</v>
@@ -2884,7 +2894,7 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B119">
         <v>0.3125</v>
@@ -2898,7 +2908,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B120">
         <v>0.15625</v>
@@ -2912,7 +2922,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B121">
         <v>7.8125E-2</v>
@@ -2926,7 +2936,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B122">
         <v>3.9063000000000001E-2</v>
@@ -2940,7 +2950,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B123">
         <v>20</v>
@@ -2954,7 +2964,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B124">
         <v>10</v>
@@ -2968,7 +2978,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B125">
         <v>5</v>
@@ -2982,7 +2992,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B126">
         <v>2.5</v>
@@ -2996,7 +3006,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B127">
         <v>1.25</v>
@@ -3010,7 +3020,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B128">
         <v>0.625</v>
@@ -3024,7 +3034,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B129">
         <v>0.3125</v>
@@ -3038,7 +3048,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B130">
         <v>0.15625</v>
@@ -3052,7 +3062,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B131">
         <v>7.8125E-2</v>
@@ -3066,7 +3076,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B132">
         <v>3.9063000000000001E-2</v>
@@ -3080,7 +3090,7 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B133">
         <v>20</v>
@@ -3094,7 +3104,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B134">
         <v>10</v>
@@ -3108,7 +3118,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B135">
         <v>5</v>
@@ -3122,7 +3132,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B136">
         <v>2.5</v>
@@ -3136,7 +3146,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B137">
         <v>1.25</v>
@@ -3150,7 +3160,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B138">
         <v>0.625</v>
@@ -3164,7 +3174,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B139">
         <v>0.3125</v>
@@ -3178,7 +3188,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B140">
         <v>0.15625</v>
@@ -3192,7 +3202,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B141">
         <v>7.8125E-2</v>
@@ -3206,7 +3216,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B142">
         <v>3.9063000000000001E-2</v>
@@ -3220,7 +3230,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B143">
         <v>20</v>
@@ -3234,7 +3244,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B144">
         <v>10</v>
@@ -3248,7 +3258,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B145">
         <v>5</v>
@@ -3262,7 +3272,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B146">
         <v>2.5</v>
@@ -3276,7 +3286,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B147">
         <v>1.25</v>
@@ -3290,7 +3300,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B148">
         <v>0.625</v>
@@ -3304,7 +3314,7 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B149">
         <v>0.3125</v>
@@ -3318,7 +3328,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B150">
         <v>0.15625</v>
@@ -3332,7 +3342,7 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B151">
         <v>7.8125E-2</v>
@@ -3346,7 +3356,7 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B152">
         <v>3.9063000000000001E-2</v>
@@ -3360,7 +3370,7 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B153">
         <v>20</v>
@@ -3374,7 +3384,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B154">
         <v>10</v>
@@ -3388,7 +3398,7 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B155">
         <v>5</v>
@@ -3402,7 +3412,7 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B156">
         <v>2.5</v>
@@ -3416,7 +3426,7 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B157">
         <v>1.25</v>
@@ -3430,7 +3440,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B158">
         <v>0.625</v>
@@ -3444,7 +3454,7 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B159">
         <v>0.3125</v>
@@ -3458,7 +3468,7 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B160">
         <v>0.15625</v>
@@ -3472,7 +3482,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B161">
         <v>7.8125E-2</v>
@@ -3486,7 +3496,7 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B162">
         <v>3.9063000000000001E-2</v>
@@ -3500,7 +3510,7 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B163">
         <v>20</v>
@@ -3514,7 +3524,7 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B164">
         <v>10</v>
@@ -3528,7 +3538,7 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B165">
         <v>5</v>
@@ -3542,7 +3552,7 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B166">
         <v>2.5</v>
@@ -3556,7 +3566,7 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B167">
         <v>1.25</v>
@@ -3570,7 +3580,7 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B168">
         <v>0.625</v>
@@ -3584,7 +3594,7 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B169">
         <v>0.3125</v>
@@ -3598,7 +3608,7 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B170">
         <v>0.15625</v>
@@ -3612,7 +3622,7 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B171">
         <v>7.8125E-2</v>
@@ -3626,7 +3636,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B172">
         <v>3.9063000000000001E-2</v>
@@ -3640,7 +3650,7 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B173">
         <v>20</v>
@@ -3654,7 +3664,7 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B174">
         <v>10</v>
@@ -3668,7 +3678,7 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B175">
         <v>5</v>
@@ -3682,7 +3692,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B176">
         <v>2.5</v>
@@ -3696,7 +3706,7 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B177">
         <v>1.25</v>
@@ -3710,7 +3720,7 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B178">
         <v>0.625</v>
@@ -3724,7 +3734,7 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B179">
         <v>0.3125</v>
@@ -3738,7 +3748,7 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B180">
         <v>0.15625</v>
@@ -3752,7 +3762,7 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B181">
         <v>7.8125E-2</v>
@@ -3766,7 +3776,7 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B182">
         <v>3.9063000000000001E-2</v>
@@ -3780,7 +3790,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B183">
         <v>20</v>
@@ -3794,7 +3804,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B184">
         <v>10</v>
@@ -3808,7 +3818,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B185">
         <v>5</v>
@@ -3822,7 +3832,7 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B186">
         <v>2.5</v>
@@ -3836,7 +3846,7 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B187">
         <v>1.25</v>
@@ -3850,7 +3860,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B188">
         <v>0.625</v>
@@ -3864,7 +3874,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B189">
         <v>0.3125</v>
@@ -3878,7 +3888,7 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B190">
         <v>0.15625</v>
@@ -3892,7 +3902,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B191">
         <v>20</v>
@@ -3906,7 +3916,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B192">
         <v>10</v>
@@ -3920,7 +3930,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B193">
         <v>5</v>
@@ -3934,7 +3944,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B194">
         <v>2.5</v>
@@ -3948,7 +3958,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B195">
         <v>1.25</v>
@@ -3962,7 +3972,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B196">
         <v>0.625</v>
@@ -3976,7 +3986,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B197">
         <v>0.3125</v>
@@ -3990,7 +4000,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B198">
         <v>0.15625</v>
@@ -4004,7 +4014,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B199">
         <v>7.8125E-2</v>
@@ -4018,7 +4028,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B200">
         <v>3.9063000000000001E-2</v>
@@ -4032,7 +4042,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B201">
         <v>7.8125E-2</v>
@@ -4046,7 +4056,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B202">
         <v>3.9063000000000001E-2</v>
@@ -4060,7 +4070,7 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B203">
         <v>20</v>
@@ -4074,7 +4084,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B204">
         <v>10</v>
@@ -4088,7 +4098,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B205">
         <v>5</v>
@@ -4102,7 +4112,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B206">
         <v>2.5</v>
@@ -4116,7 +4126,7 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B207">
         <v>1.25</v>
@@ -4130,7 +4140,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B208">
         <v>0.625</v>
@@ -4144,7 +4154,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B209">
         <v>0.3125</v>
@@ -4158,7 +4168,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B210">
         <v>0.15625</v>
@@ -4172,7 +4182,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B211">
         <v>7.8125E-2</v>
@@ -4186,7 +4196,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B212">
         <v>3.9063000000000001E-2</v>
@@ -4200,7 +4210,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B213">
         <v>20</v>
@@ -4214,7 +4224,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B214">
         <v>10</v>
@@ -4228,7 +4238,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B215">
         <v>5</v>
@@ -4242,7 +4252,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B216">
         <v>2.5</v>
@@ -4256,7 +4266,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B217">
         <v>1.25</v>
@@ -4270,7 +4280,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B218">
         <v>0.625</v>
@@ -4284,7 +4294,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B219">
         <v>0.3125</v>
@@ -4298,7 +4308,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B220">
         <v>0.15625</v>
@@ -4312,7 +4322,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B221">
         <v>7.8125E-2</v>
@@ -4326,7 +4336,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B222">
         <v>3.9063000000000001E-2</v>
@@ -4340,7 +4350,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B223">
         <v>20</v>
@@ -4354,7 +4364,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B224">
         <v>10</v>
@@ -4368,7 +4378,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B225">
         <v>5</v>
@@ -4382,7 +4392,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B226">
         <v>2.5</v>
@@ -4396,7 +4406,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B227">
         <v>1.25</v>
@@ -4410,7 +4420,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B228">
         <v>0.625</v>
@@ -4424,7 +4434,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B229">
         <v>0.3125</v>
@@ -4438,7 +4448,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B230">
         <v>0.15625</v>
@@ -4452,7 +4462,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B231">
         <v>7.8125E-2</v>
@@ -4466,7 +4476,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B232">
         <v>3.9063000000000001E-2</v>
@@ -5721,7 +5731,7 @@
         <v>-15.846</v>
       </c>
       <c r="D321" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E321">
         <v>289</v>

</xml_diff>

<commit_message>
SEL: adding note about config addition
</commit_message>
<xml_diff>
--- a/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
+++ b/public/src/modules/GenericDataParser/spec/specFiles/explicit_ACAS_format.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="64">
   <si>
     <t>Format</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Hill slope</t>
-  </si>
-  <si>
-    <t>spilled</t>
   </si>
   <si>
     <t>flagged</t>
@@ -398,6 +395,15 @@
   <si>
     <t>CMPD-0000011-01A</t>
   </si>
+  <si>
+    <t>on load</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
 </sst>
 </file>
 
@@ -497,10 +503,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -516,14 +524,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -856,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H432"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -886,15 +896,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -913,7 +923,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -933,54 +943,54 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1011,7 +1021,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1037,7 +1047,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1063,7 +1073,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1089,7 +1099,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1115,7 +1125,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -1141,7 +1151,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -1167,7 +1177,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -1193,7 +1203,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1219,7 +1229,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1245,7 +1255,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -1271,7 +1281,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1297,7 +1307,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1326,31 +1336,31 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1379,52 +1389,61 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1436,13 +1455,16 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1456,10 +1478,10 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1470,16 +1492,19 @@
         <v>89.825999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>28</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1493,10 +1518,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1510,10 +1535,10 @@
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1527,10 +1552,10 @@
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1544,10 +1569,10 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1561,10 +1586,10 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1578,10 +1603,10 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1595,10 +1620,10 @@
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1612,10 +1637,10 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1629,10 +1654,10 @@
         <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1646,10 +1671,10 @@
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -1663,10 +1688,10 @@
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -1680,10 +1705,10 @@
         <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -1697,10 +1722,10 @@
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1714,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1731,7 +1756,7 @@
         <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1748,7 +1773,7 @@
         <v>18</v>
       </c>
       <c r="F50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1765,7 +1790,7 @@
         <v>19</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1782,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1799,7 +1824,7 @@
         <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1816,7 +1841,7 @@
         <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1833,7 +1858,7 @@
         <v>23</v>
       </c>
       <c r="F55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1850,7 +1875,7 @@
         <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1867,7 +1892,7 @@
         <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1884,7 +1909,7 @@
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1901,7 +1926,7 @@
         <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1918,7 +1943,7 @@
         <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1935,7 +1960,7 @@
         <v>29</v>
       </c>
       <c r="F61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1952,7 +1977,7 @@
         <v>30</v>
       </c>
       <c r="F62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1969,7 +1994,7 @@
         <v>31</v>
       </c>
       <c r="F63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1986,7 +2011,7 @@
         <v>32</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2003,7 +2028,7 @@
         <v>33</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2020,7 +2045,7 @@
         <v>34</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2037,7 +2062,7 @@
         <v>35</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2054,7 +2079,7 @@
         <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2071,7 +2096,7 @@
         <v>37</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2088,7 +2113,7 @@
         <v>38</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2105,7 +2130,7 @@
         <v>39</v>
       </c>
       <c r="F71" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2122,7 +2147,7 @@
         <v>40</v>
       </c>
       <c r="F72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2139,7 +2164,7 @@
         <v>41</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2156,7 +2181,7 @@
         <v>42</v>
       </c>
       <c r="F74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2173,7 +2198,7 @@
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2190,7 +2215,7 @@
         <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2207,7 +2232,7 @@
         <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2224,7 +2249,7 @@
         <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2241,7 +2266,7 @@
         <v>47</v>
       </c>
       <c r="F79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2258,7 +2283,7 @@
         <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2275,7 +2300,7 @@
         <v>49</v>
       </c>
       <c r="F81" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2292,7 +2317,7 @@
         <v>50</v>
       </c>
       <c r="F82" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2309,7 +2334,7 @@
         <v>51</v>
       </c>
       <c r="F83" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2326,7 +2351,7 @@
         <v>52</v>
       </c>
       <c r="F84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2343,7 +2368,7 @@
         <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2360,7 +2385,7 @@
         <v>54</v>
       </c>
       <c r="F86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2377,7 +2402,7 @@
         <v>55</v>
       </c>
       <c r="F87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2394,7 +2419,7 @@
         <v>56</v>
       </c>
       <c r="F88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2411,7 +2436,7 @@
         <v>57</v>
       </c>
       <c r="F89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2428,7 +2453,7 @@
         <v>58</v>
       </c>
       <c r="F90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2445,7 +2470,7 @@
         <v>59</v>
       </c>
       <c r="F91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2462,7 +2487,7 @@
         <v>60</v>
       </c>
       <c r="F92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2479,7 +2504,7 @@
         <v>61</v>
       </c>
       <c r="F93" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2496,7 +2521,7 @@
         <v>62</v>
       </c>
       <c r="F94" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2513,7 +2538,7 @@
         <v>63</v>
       </c>
       <c r="F95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2530,7 +2555,7 @@
         <v>64</v>
       </c>
       <c r="F96" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2547,7 +2572,7 @@
         <v>65</v>
       </c>
       <c r="F97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2564,7 +2589,7 @@
         <v>66</v>
       </c>
       <c r="F98" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2581,7 +2606,7 @@
         <v>67</v>
       </c>
       <c r="F99" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2598,7 +2623,7 @@
         <v>68</v>
       </c>
       <c r="F100" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2615,7 +2640,7 @@
         <v>69</v>
       </c>
       <c r="F101" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2632,7 +2657,7 @@
         <v>70</v>
       </c>
       <c r="F102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2649,7 +2674,7 @@
         <v>71</v>
       </c>
       <c r="F103" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2666,7 +2691,7 @@
         <v>72</v>
       </c>
       <c r="F104" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2683,7 +2708,7 @@
         <v>73</v>
       </c>
       <c r="F105" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2700,7 +2725,7 @@
         <v>74</v>
       </c>
       <c r="F106" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2717,7 +2742,7 @@
         <v>75</v>
       </c>
       <c r="F107" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2734,7 +2759,7 @@
         <v>76</v>
       </c>
       <c r="F108" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2751,7 +2776,7 @@
         <v>77</v>
       </c>
       <c r="F109" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2768,7 +2793,7 @@
         <v>78</v>
       </c>
       <c r="F110" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2785,7 +2810,7 @@
         <v>79</v>
       </c>
       <c r="F111" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2802,7 +2827,7 @@
         <v>80</v>
       </c>
       <c r="F112" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2819,7 +2844,7 @@
         <v>81</v>
       </c>
       <c r="F113" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -5731,7 +5756,7 @@
         <v>-15.846</v>
       </c>
       <c r="D321" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E321">
         <v>289</v>

</xml_diff>